<commit_message>
TMT0072172_TMT0072174_VerifyBothPrimaryAndNonPrimaryAttendeeCanSendNotificationFromSF - Final - 9th Sep 2024
</commit_message>
<xml_diff>
--- a/TestData/TMTC0032668_VerifyBothPrimaryAndNonPrimaryAttendeeCanSendNotificationFromSF.xlsx
+++ b/TestData/TMTC0032668_VerifyBothPrimaryAndNonPrimaryAttendeeCanSendNotificationFromSF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5BD3B59-2B54-4858-835C-5075AC116024}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20358878-976A-4B39-9A7E-A1B3C6CFAC7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
   <si>
     <t>Users</t>
   </si>
@@ -124,16 +124,13 @@
   </si>
   <si>
     <t>Email ID</t>
-  </si>
-  <si>
-    <t>Sahil.Mittal0207@hl.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,14 +148,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -181,20 +170,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -676,7 +662,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1F0BEF1-BEAB-4FB8-98E8-E9DD69129D4A}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -686,14 +674,11 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>28</v>
+      <c r="A2" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{06CBCBDF-D107-49CF-842B-16B253280570}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>